<commit_message>
update list of thigns to avoid and keep doing in spring report
</commit_message>
<xml_diff>
--- a/Team03Report.xlsx
+++ b/Team03Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python Project\SSW555\CS555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0426A678-2C3D-46DC-9D5A-D1DD7DDFCA75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84945D77-2211-4285-83A4-DDDB0766B968}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="209">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -684,6 +684,24 @@
   </si>
   <si>
     <t>https://github.com/Shaunak1857/CS555_Project</t>
+  </si>
+  <si>
+    <t>Pre sprint planning meeting to discuss implementation pattern</t>
+  </si>
+  <si>
+    <t>End of sprint code review</t>
+  </si>
+  <si>
+    <t>List of common formatting in the code to keep style the same</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre sprint meeting should've been earlier; people started working in different directions before we decided on a infrastructure. </t>
+  </si>
+  <si>
+    <t>Mid sprint code review to make sure everyone is on the same page and catch early bugs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential code refactor into different files to reduce file size. </t>
   </si>
 </sst>
 </file>
@@ -2240,7 +2258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="150" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -2498,10 +2516,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2782,10 +2800,36 @@
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="5" t="s">
+      <c r="C16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="5" t="s">
         <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
report and unitTest.py up-to-date
</commit_message>
<xml_diff>
--- a/Team03Report.xlsx
+++ b/Team03Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python Project\SSW555\CS555_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunaksaklikar/Documents/cs555/finalProject/CS555_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84945D77-2211-4285-83A4-DDDB0766B968}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F00D35-EFEB-524F-97A0-A6A76EB1BE2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="210">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -668,9 +668,6 @@
     <t>yzhao118@stevens.edu</t>
   </si>
   <si>
-    <t>InProgress</t>
-  </si>
-  <si>
     <t>z1103246</t>
   </si>
   <si>
@@ -702,6 +699,12 @@
   </si>
   <si>
     <t xml:space="preserve">Potential code refactor into different files to reduce file size. </t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In-progress</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1034,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42796</c:v>
@@ -1059,6 +1062,9 @@
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1093,7 +1099,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1159,13 +1165,19 @@
             <c:numRef>
               <c:f>Burndown!$A$2:$A$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40442</c:v>
+                  <c:v>42810</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40455</c:v>
+                  <c:v>42824</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42838</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42852</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1177,10 +1189,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1212,7 +1221,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2074,16 +2083,16 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.375" customWidth="1"/>
-    <col min="3" max="3" width="13.375" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="4" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="6" width="14.125" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2103,7 +2112,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>178</v>
       </c>
@@ -2117,13 +2126,13 @@
         <v>188</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>181</v>
       </c>
@@ -2137,13 +2146,13 @@
         <v>190</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F4" s="21" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>184</v>
       </c>
@@ -2157,13 +2166,13 @@
         <v>196</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>187</v>
       </c>
@@ -2177,18 +2186,18 @@
         <v>189</v>
       </c>
       <c r="E6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F6" s="21" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2215,16 +2224,16 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.875" customWidth="1"/>
-    <col min="2" max="2" width="16.125" customWidth="1"/>
-    <col min="3" max="3" width="22.625" customWidth="1"/>
-    <col min="4" max="4" width="10.625" customWidth="1"/>
-    <col min="5" max="5" width="12.125" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2241,10 +2250,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C3" s="1"/>
     </row>
   </sheetData>
@@ -2259,51 +2268,51 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="7"/>
-    <col min="2" max="2" width="17.625" customWidth="1"/>
-    <col min="3" max="3" width="21.875" customWidth="1"/>
-    <col min="4" max="4" width="23.125" customWidth="1"/>
-    <col min="5" max="5" width="16.125" customWidth="1"/>
-    <col min="6" max="6" width="24.125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="25.375" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -2326,7 +2335,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -2342,28 +2351,32 @@
       <c r="F15" s="13"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>163</v>
       </c>
       <c r="B16" s="12">
         <v>42810</v>
       </c>
-      <c r="C16" s="13"/>
+      <c r="C16" s="13">
+        <v>32</v>
+      </c>
       <c r="D16">
         <f>C15-C16</f>
-        <v>42</v>
-      </c>
-      <c r="E16" s="13"/>
+        <v>10</v>
+      </c>
+      <c r="E16" s="13">
+        <v>1225</v>
+      </c>
       <c r="F16" s="13">
         <v>120</v>
       </c>
       <c r="G16" s="9">
         <f>(E16-E15)/F16*60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>612.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>164</v>
       </c>
@@ -2373,7 +2386,7 @@
       <c r="C17" s="13"/>
       <c r="D17">
         <f t="shared" ref="D17:D19" si="0">C16-C17</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="14">
@@ -2381,10 +2394,10 @@
       </c>
       <c r="G17" s="9">
         <f t="shared" ref="G17:G19" si="1">(E17-E16)/F17*60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-544.44444444444446</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>165</v>
       </c>
@@ -2405,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>166</v>
       </c>
@@ -2437,23 +2450,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="25.875" customWidth="1"/>
-    <col min="3" max="3" width="21.375" customWidth="1"/>
-    <col min="4" max="4" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="16.375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2473,37 +2486,44 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>40442</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="12">
+        <v>42810</v>
       </c>
       <c r="B2">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>40455</v>
-      </c>
-      <c r="B3">
-        <v>30</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="12">
+        <v>42824</v>
       </c>
       <c r="C3">
         <f>B2-B3</f>
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D3">
-        <v>250</v>
+        <v>1225</v>
       </c>
       <c r="E3">
         <v>120</v>
       </c>
       <c r="F3" s="9">
         <f>(D3-D2)/E3*60</f>
-        <v>125.00000000000001</v>
+        <v>612.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="12">
+        <v>42838</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="12">
+        <v>42852</v>
       </c>
     </row>
   </sheetData>
@@ -2518,23 +2538,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.625" customWidth="1"/>
-    <col min="2" max="2" width="33.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.875" customWidth="1"/>
-    <col min="6" max="6" width="14.125" customWidth="1"/>
-    <col min="7" max="7" width="12.875" customWidth="1"/>
-    <col min="8" max="8" width="16.125" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" customWidth="1"/>
     <col min="9" max="9" width="20" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2563,7 +2583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2574,7 +2594,7 @@
         <v>187</v>
       </c>
       <c r="D2" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="E2">
         <v>130</v>
@@ -2582,8 +2602,17 @@
       <c r="F2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>130</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="7">
+        <v>42808</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2594,7 +2623,7 @@
         <v>178</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="E3">
         <v>150</v>
@@ -2602,8 +2631,17 @@
       <c r="F3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>150</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="7">
+        <v>42808</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2614,7 +2652,7 @@
         <v>184</v>
       </c>
       <c r="D4" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="E4">
         <v>200</v>
@@ -2632,7 +2670,7 @@
         <v>42801</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2643,7 +2681,7 @@
         <v>184</v>
       </c>
       <c r="D5" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="E5">
         <v>130</v>
@@ -2657,8 +2695,11 @@
       <c r="H5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I5" s="7">
+        <v>42808</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2669,7 +2710,7 @@
         <v>181</v>
       </c>
       <c r="D6" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="E6">
         <v>170</v>
@@ -2677,8 +2718,17 @@
       <c r="F6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>150</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6" s="7">
+        <v>42810</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2689,7 +2739,7 @@
         <v>181</v>
       </c>
       <c r="D7" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="E7">
         <v>100</v>
@@ -2697,8 +2747,17 @@
       <c r="F7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>120</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7" s="7">
+        <v>42808</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2709,7 +2768,7 @@
         <v>187</v>
       </c>
       <c r="D8" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="E8">
         <v>150</v>
@@ -2717,8 +2776,17 @@
       <c r="F8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>130</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8" s="7">
+        <v>42809</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2729,7 +2797,7 @@
         <v>184</v>
       </c>
       <c r="D9" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="E9">
         <v>180</v>
@@ -2747,7 +2815,7 @@
         <v>42803</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2758,7 +2826,7 @@
         <v>178</v>
       </c>
       <c r="D10" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="E10">
         <v>111</v>
@@ -2766,8 +2834,17 @@
       <c r="F10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>150</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10" s="7">
+        <v>42809</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2778,7 +2855,7 @@
         <v>178</v>
       </c>
       <c r="D11" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="E11">
         <v>100</v>
@@ -2786,50 +2863,59 @@
       <c r="F11">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>110</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11" s="7">
+        <v>42810</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C17" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C18" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" ht="14" x14ac:dyDescent="0.15">
       <c r="B21" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C22" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C23" t="s">
         <v>207</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2841,15 +2927,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2876,6 +2965,206 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2">
+        <v>120</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E3">
+        <v>130</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E4">
+        <v>150</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5">
+        <v>125</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E6">
+        <v>135</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7" t="s">
+        <v>209</v>
+      </c>
+      <c r="E7">
+        <v>122</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" t="s">
+        <v>209</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" t="s">
+        <v>178</v>
+      </c>
+      <c r="D9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E9">
+        <v>110</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" t="s">
+        <v>209</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11" t="s">
+        <v>209</v>
+      </c>
+      <c r="E11">
+        <v>150</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2893,9 +3182,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2938,9 +3227,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2979,17 +3268,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -3000,7 +3289,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3011,7 +3300,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -3022,7 +3311,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3033,7 +3322,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3044,7 +3333,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3055,7 +3344,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -3066,7 +3355,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3077,7 +3366,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3088,7 +3377,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3099,7 +3388,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3110,7 +3399,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3121,7 +3410,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -3132,7 +3421,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -3143,7 +3432,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -3154,7 +3443,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -3165,7 +3454,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -3176,7 +3465,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -3187,7 +3476,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -3198,7 +3487,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -3209,7 +3498,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -3220,7 +3509,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -3231,7 +3520,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -3242,7 +3531,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -3253,7 +3542,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -3264,7 +3553,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -3275,7 +3564,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="85" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -3286,7 +3575,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -3297,7 +3586,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -3308,7 +3597,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -3319,7 +3608,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -3330,7 +3619,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -3341,7 +3630,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -3352,7 +3641,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -3363,7 +3652,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -3374,7 +3663,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -3385,7 +3674,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -3396,7 +3685,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -3407,7 +3696,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -3418,7 +3707,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -3429,7 +3718,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -3440,7 +3729,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -3451,7 +3740,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
Added US27 and US30 and corresponding test cases
</commit_message>
<xml_diff>
--- a/Team03Report.xlsx
+++ b/Team03Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunaksaklikar/Documents/cs555/finalProject/CS555_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python Project\SSW555\CS555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FDC408-6245-5F44-BFB8-0ED0E3EAB8A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726B8848-4651-4BBB-BFEC-8ECB6E1854F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -1035,7 +1035,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42796</c:v>
@@ -1103,7 +1103,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1169,7 +1169,7 @@
             <c:numRef>
               <c:f>Burndown!$A$2:$A$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42810</c:v>
@@ -1228,7 +1228,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2090,16 +2090,16 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
     <col min="4" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>178</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>181</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>184</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>187</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2231,16 +2231,16 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="2" max="2" width="16.125" customWidth="1"/>
+    <col min="3" max="3" width="22.625" customWidth="1"/>
+    <col min="4" max="4" width="10.625" customWidth="1"/>
+    <col min="5" max="5" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2257,10 +2257,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C3" s="1"/>
     </row>
   </sheetData>
@@ -2278,48 +2278,48 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="6" max="6" width="24.1640625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="7"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
+    <col min="3" max="3" width="21.875" customWidth="1"/>
+    <col min="4" max="4" width="23.125" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
+    <col min="6" max="6" width="24.125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="25.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -2358,7 +2358,7 @@
       <c r="F15" s="13"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>612.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>164</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>258.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>165</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>-677.25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>166</v>
       </c>
@@ -2467,17 +2467,17 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="25.875" customWidth="1"/>
+    <col min="3" max="3" width="21.375" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="16.375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
         <v>42810</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>42824</v>
       </c>
@@ -2530,12 +2530,12 @@
         <v>290.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>42838</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>42852</v>
       </c>
@@ -2556,19 +2556,19 @@
       <selection activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="33.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.875" customWidth="1"/>
+    <col min="6" max="6" width="14.125" customWidth="1"/>
+    <col min="7" max="7" width="12.875" customWidth="1"/>
+    <col min="8" max="8" width="16.125" customWidth="1"/>
     <col min="9" max="9" width="20" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>42808</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>42808</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>42801</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>42808</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>42810</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>42808</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>42809</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>42803</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>42809</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2887,16 +2887,16 @@
         <v>42810</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
@@ -2904,17 +2904,17 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
         <v>32</v>
       </c>
@@ -2922,12 +2922,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>207</v>
       </c>
@@ -2943,16 +2943,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>11</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>42824</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>12</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>42821</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>13</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>42824</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>14</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>42824</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>15</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>42822</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>16</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>42822</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>17</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>42821</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>18</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>42822</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>19</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>42824</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20</v>
       </c>
@@ -3282,17 +3282,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>21</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>22</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>23</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>24</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>25</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>26</v>
       </c>
@@ -3440,8 +3440,17 @@
       <c r="F7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7" s="12">
+        <v>42826</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>27</v>
       </c>
@@ -3461,7 +3470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>28</v>
       </c>
@@ -3481,7 +3490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>29</v>
       </c>
@@ -3501,7 +3510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>30</v>
       </c>
@@ -3519,6 +3528,15 @@
       </c>
       <c r="F11">
         <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="12">
+        <v>42826</v>
       </c>
     </row>
   </sheetData>
@@ -3535,9 +3553,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3576,17 +3594,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -3597,7 +3615,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3608,7 +3626,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -3619,7 +3637,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3630,7 +3648,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3641,7 +3659,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3652,7 +3670,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -3663,7 +3681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3674,7 +3692,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3685,7 +3703,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3696,7 +3714,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3707,7 +3725,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3718,7 +3736,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -3729,7 +3747,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -3740,7 +3758,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -3751,7 +3769,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -3762,7 +3780,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -3773,7 +3791,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -3784,7 +3802,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -3795,7 +3813,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -3806,7 +3824,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -3817,7 +3835,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -3828,7 +3846,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -3839,7 +3857,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -3850,7 +3868,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -3861,7 +3879,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -3872,7 +3890,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="85" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -3883,7 +3901,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -3894,7 +3912,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -3905,7 +3923,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -3916,7 +3934,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -3927,7 +3945,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -3938,7 +3956,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -3949,7 +3967,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -3960,7 +3978,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -3971,7 +3989,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -3982,7 +4000,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -3993,7 +4011,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -4004,7 +4022,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -4015,7 +4033,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -4026,7 +4044,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -4037,7 +4055,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -4048,7 +4066,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
loc remaingin in the report
</commit_message>
<xml_diff>
--- a/Team03Report.xlsx
+++ b/Team03Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunaksaklikar/Documents/cs555/finalProject/CS555_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B68CD4-E043-9C4D-895F-9445CC313333}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93095BB-6C27-9D4E-BF77-77389C6D55D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="209">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1067,6 +1067,9 @@
                 <c:pt idx="2">
                   <c:v>22</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1194,6 +1197,12 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2083,7 +2092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -2272,7 +2281,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A8" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2412,10 +2421,12 @@
       <c r="B18" s="12">
         <v>42838</v>
       </c>
-      <c r="C18" s="13"/>
+      <c r="C18" s="13">
+        <v>12</v>
+      </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="14">
@@ -2438,7 +2449,7 @@
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="14">
@@ -2461,7 +2472,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2531,10 +2542,22 @@
       <c r="A4" s="12">
         <v>42838</v>
       </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="12">
         <v>42852</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2941,7 +2964,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="E2" sqref="E2:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3279,8 +3302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3344,7 +3367,7 @@
         <v>3</v>
       </c>
       <c r="I2" s="12">
-        <v>42826</v>
+        <v>42838</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -3373,7 +3396,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="12">
-        <v>42826</v>
+        <v>42838</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -3402,7 +3425,7 @@
         <v>4</v>
       </c>
       <c r="I4" s="12">
-        <v>42826</v>
+        <v>42838</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
@@ -3431,7 +3454,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="12">
-        <v>42826</v>
+        <v>42838</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
@@ -3460,7 +3483,7 @@
         <v>3</v>
       </c>
       <c r="I6" s="12">
-        <v>42826</v>
+        <v>42838</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
@@ -3489,7 +3512,7 @@
         <v>4</v>
       </c>
       <c r="I7" s="12">
-        <v>42826</v>
+        <v>42838</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
@@ -3518,7 +3541,7 @@
         <v>2</v>
       </c>
       <c r="I8" s="12">
-        <v>42826</v>
+        <v>42838</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
@@ -3547,7 +3570,7 @@
         <v>3</v>
       </c>
       <c r="I9" s="12">
-        <v>42826</v>
+        <v>42838</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
@@ -3576,7 +3599,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="12">
-        <v>42826</v>
+        <v>42838</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -3605,7 +3628,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="12">
-        <v>42826</v>
+        <v>42838</v>
       </c>
     </row>
   </sheetData>
@@ -3616,13 +3639,16 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
@@ -3651,6 +3677,354 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2">
+        <v>120</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="12">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E3">
+        <v>130</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>130</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3" s="12">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4">
+        <v>150</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>110</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4" s="12">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5">
+        <v>125</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>120</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5" s="12">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6">
+        <v>135</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="12">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" t="s">
+        <v>208</v>
+      </c>
+      <c r="E7">
+        <v>122</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>14</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7" s="12">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>200</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8" s="12">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E9">
+        <v>110</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9" s="12">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>120</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10" s="12">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" t="s">
+        <v>187</v>
+      </c>
+      <c r="D11" t="s">
+        <v>208</v>
+      </c>
+      <c r="E11">
+        <v>150</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>160</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11" s="12">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" t="s">
+        <v>208</v>
+      </c>
+      <c r="E12">
+        <v>120</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>120</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12" s="12">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" t="s">
+        <v>208</v>
+      </c>
+      <c r="E13">
+        <v>130</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>140</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" s="12">
+        <v>42852</v>
       </c>
     </row>
   </sheetData>
@@ -3663,8 +4037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A30" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>